<commit_message>
Mon ERD and Pitchbook Update
</commit_message>
<xml_diff>
--- a/Rodgers_ERD.xlsx
+++ b/Rodgers_ERD.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodge\Documents\sql-challenge\EmployeeSQL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodge\Documents\sql-challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32486C4A-E3BE-4E16-A385-297992125FDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D4355D-5B01-44AD-98E1-5B38656B3507}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1178E2C9-5C18-4B10-8129-0E9588271537}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="23">
   <si>
     <t>dept_no</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Employee_Manager</t>
   </si>
   <si>
-    <t>manager</t>
-  </si>
-  <si>
     <t>emp_title_id</t>
   </si>
   <si>
@@ -96,31 +93,7 @@
     <t>FK</t>
   </si>
   <si>
-    <t>Boolean (default true)</t>
-  </si>
-  <si>
     <t>RODGERS ERD FOR SQL-CHALLENGE</t>
-  </si>
-  <si>
-    <t>title_item</t>
-  </si>
-  <si>
-    <t>SERIAL</t>
-  </si>
-  <si>
-    <t>junction_item</t>
-  </si>
-  <si>
-    <t>manager_item</t>
-  </si>
-  <si>
-    <t>department_item</t>
-  </si>
-  <si>
-    <t>salary_item</t>
-  </si>
-  <si>
-    <t>empl_item</t>
   </si>
 </sst>
 </file>
@@ -151,7 +124,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,12 +134,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -306,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -319,12 +286,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -455,7 +419,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>281940</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -555,7 +519,7 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -656,13 +620,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>121920</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>106680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>220980</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1002,10 +966,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C0F0DF4-23BC-4349-BF66-E85E31894105}">
-  <dimension ref="B1:N22"/>
+  <dimension ref="B1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1026,24 +990,24 @@
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B4" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="11"/>
       <c r="G4" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="11"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="18" t="s">
-        <v>18</v>
+      <c r="B5" s="15" t="s">
+        <v>17</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>3</v>
@@ -1051,19 +1015,19 @@
       <c r="D5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="18" t="s">
-        <v>10</v>
+      <c r="G5" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>3</v>
@@ -1080,15 +1044,11 @@
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="17"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="14"/>
       <c r="G7" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>3</v>
@@ -1097,7 +1057,7 @@
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="G8" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>3</v>
@@ -1106,12 +1066,12 @@
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="8"/>
       <c r="G9" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>3</v>
@@ -1129,7 +1089,7 @@
         <v>4</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>3</v>
@@ -1138,14 +1098,14 @@
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="6"/>
       <c r="G11" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>3</v>
@@ -1153,20 +1113,12 @@
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="17"/>
-      <c r="G12" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="H12" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="I12" s="17"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="14"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="14"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
       <c r="L13" s="9" t="s">
@@ -1194,86 +1146,69 @@
         <v>3</v>
       </c>
       <c r="N15" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="L16" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="M16" s="13" t="s">
-        <v>23</v>
-      </c>
+      <c r="L16" s="12"/>
+      <c r="M16" s="13"/>
       <c r="N16" s="14"/>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="L17" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="M17" s="16"/>
-      <c r="N17" s="17"/>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B18" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="11"/>
+      <c r="L18" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="M18" s="10"/>
+      <c r="N18" s="11"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B19" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="11"/>
-      <c r="L19" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="M19" s="10"/>
-      <c r="N19" s="11"/>
+      <c r="B19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="L19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="M19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="N19" s="6" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B20" s="4" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="6"/>
+        <v>3</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="L20" s="4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M20" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="N20" s="6" t="s">
-        <v>4</v>
-      </c>
+      <c r="N20" s="6"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B21" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L21" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="M21" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="N21" s="6"/>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B22" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="17"/>
-      <c r="L22" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="M22" s="16"/>
-      <c r="N22" s="17"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="14"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>